<commit_message>
Added quiz seed data
</commit_message>
<xml_diff>
--- a/app/assets/data/AnswerChoices.xlsx
+++ b/app/assets/data/AnswerChoices.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26009"/>
-  <workbookPr showInkAnnotation="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SrinjoyMajumdar/Documents/AtsaCorp/ImagineDragons/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="1940" windowWidth="27360" windowHeight="15740" tabRatio="500"/>
+    <workbookView xWindow="9180" yWindow="840" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="52">
   <si>
     <t>a</t>
   </si>
@@ -48,16 +43,164 @@
   </si>
   <si>
     <t>answer 4</t>
+  </si>
+  <si>
+    <t>Jupiter</t>
+  </si>
+  <si>
+    <t>Earth</t>
+  </si>
+  <si>
+    <t>Venus</t>
+  </si>
+  <si>
+    <t>Mars</t>
+  </si>
+  <si>
+    <t>Andromeda</t>
+  </si>
+  <si>
+    <t>Milky Way</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pinwheel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cigar </t>
+  </si>
+  <si>
+    <t>Sun</t>
+  </si>
+  <si>
+    <t>Moon</t>
+  </si>
+  <si>
+    <t>Orion</t>
+  </si>
+  <si>
+    <t>Delphinus</t>
+  </si>
+  <si>
+    <t>Scorpius</t>
+  </si>
+  <si>
+    <t>Pisces</t>
+  </si>
+  <si>
+    <t>The Earth's axis is tilted</t>
+  </si>
+  <si>
+    <t>The Sun is the center of the universe</t>
+  </si>
+  <si>
+    <t>The Earth's orbit around the Sun is elliptical</t>
+  </si>
+  <si>
+    <t>The Sun gets weaker in the Winter</t>
+  </si>
+  <si>
+    <t>0.05°</t>
+  </si>
+  <si>
+    <t>0.1°</t>
+  </si>
+  <si>
+    <t>0.25°</t>
+  </si>
+  <si>
+    <t>0.5°</t>
+  </si>
+  <si>
+    <t>Equator</t>
+  </si>
+  <si>
+    <t>Pole</t>
+  </si>
+  <si>
+    <t>Terminator</t>
+  </si>
+  <si>
+    <t>Orbit</t>
+  </si>
+  <si>
+    <t>New Moon</t>
+  </si>
+  <si>
+    <t>First Quarter</t>
+  </si>
+  <si>
+    <t>Full Moon</t>
+  </si>
+  <si>
+    <t>Third Quarter</t>
+  </si>
+  <si>
+    <t>Darkest Part of Shadow cast by Moon</t>
+  </si>
+  <si>
+    <t>The large outer part of the moon's shadow</t>
+  </si>
+  <si>
+    <t>Total Eclipse</t>
+  </si>
+  <si>
+    <t>Annular Eclipse</t>
+  </si>
+  <si>
+    <t>The center of the Sun</t>
+  </si>
+  <si>
+    <t>The Photospher</t>
+  </si>
+  <si>
+    <t>The Convective Zone</t>
+  </si>
+  <si>
+    <t>Lunar Eclipse</t>
+  </si>
+  <si>
+    <t>Partial Eclipse</t>
+  </si>
+  <si>
+    <t>Diamond Ring Effect</t>
+  </si>
+  <si>
+    <t>Baily's Beads</t>
+  </si>
+  <si>
+    <t>Lunar Silhouette</t>
+  </si>
+  <si>
+    <t>Partial Light Effect</t>
+  </si>
+  <si>
+    <t>The extended outer atmosphere of the Sun</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -80,13 +223,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -142,7 +297,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -177,7 +332,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -354,7 +509,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -364,13 +519,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77:D80"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1">
         <v>1</v>
       </c>
@@ -378,13 +533,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>2</v>
       </c>
@@ -392,13 +547,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>3</v>
       </c>
@@ -406,13 +561,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>4</v>
       </c>
@@ -420,13 +575,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>5</v>
       </c>
@@ -434,13 +589,13 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>6</v>
       </c>
@@ -448,13 +603,13 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>7</v>
       </c>
@@ -462,13 +617,13 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>8</v>
       </c>
@@ -476,13 +631,13 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>9</v>
       </c>
@@ -490,13 +645,13 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>10</v>
       </c>
@@ -504,13 +659,13 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>11</v>
       </c>
@@ -518,13 +673,13 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>12</v>
       </c>
@@ -532,69 +687,69 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>13</v>
       </c>
       <c r="B13">
         <v>4</v>
       </c>
-      <c r="C13" t="s">
-        <v>4</v>
+      <c r="C13">
+        <v>68</v>
       </c>
       <c r="D13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>14</v>
       </c>
       <c r="B14">
         <v>4</v>
       </c>
-      <c r="C14" t="s">
-        <v>5</v>
+      <c r="C14">
+        <v>78</v>
       </c>
       <c r="D14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>15</v>
       </c>
       <c r="B15">
         <v>4</v>
       </c>
-      <c r="C15" t="s">
-        <v>6</v>
+      <c r="C15">
+        <v>84</v>
       </c>
       <c r="D15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>16</v>
       </c>
       <c r="B16">
         <v>4</v>
       </c>
-      <c r="C16" t="s">
-        <v>7</v>
+      <c r="C16">
+        <v>88</v>
       </c>
       <c r="D16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>17</v>
       </c>
@@ -602,13 +757,13 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>18</v>
       </c>
@@ -616,13 +771,13 @@
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>19</v>
       </c>
@@ -630,13 +785,13 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>20</v>
       </c>
@@ -644,13 +799,13 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>21</v>
       </c>
@@ -658,13 +813,13 @@
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D21" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>22</v>
       </c>
@@ -672,13 +827,13 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D22" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>23</v>
       </c>
@@ -686,13 +841,13 @@
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>24</v>
       </c>
@@ -700,13 +855,13 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D24" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>25</v>
       </c>
@@ -714,13 +869,13 @@
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D25" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>26</v>
       </c>
@@ -728,13 +883,13 @@
         <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="D26" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>27</v>
       </c>
@@ -742,13 +897,13 @@
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D27" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>28</v>
       </c>
@@ -756,13 +911,13 @@
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="D28" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>29</v>
       </c>
@@ -770,13 +925,13 @@
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="D29" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>30</v>
       </c>
@@ -784,13 +939,13 @@
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="D30" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>31</v>
       </c>
@@ -798,13 +953,13 @@
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="D31" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>32</v>
       </c>
@@ -812,13 +967,13 @@
         <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="D32" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>33</v>
       </c>
@@ -826,13 +981,13 @@
         <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D33" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>34</v>
       </c>
@@ -840,13 +995,13 @@
         <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="D34" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>35</v>
       </c>
@@ -854,13 +1009,13 @@
         <v>9</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D35" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>36</v>
       </c>
@@ -868,13 +1023,13 @@
         <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="D36" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>37</v>
       </c>
@@ -882,13 +1037,13 @@
         <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D37" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>38</v>
       </c>
@@ -896,13 +1051,13 @@
         <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="D38" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>39</v>
       </c>
@@ -910,13 +1065,13 @@
         <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D39" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40">
         <v>40</v>
       </c>
@@ -924,13 +1079,13 @@
         <v>10</v>
       </c>
       <c r="C40" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="D40" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>41</v>
       </c>
@@ -938,13 +1093,13 @@
         <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="D41" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>42</v>
       </c>
@@ -952,13 +1107,13 @@
         <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="D42" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>43</v>
       </c>
@@ -966,13 +1121,13 @@
         <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="D43" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>44</v>
       </c>
@@ -980,13 +1135,13 @@
         <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="D44" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>45</v>
       </c>
@@ -994,13 +1149,13 @@
         <v>12</v>
       </c>
       <c r="C45" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="D45" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46">
         <v>46</v>
       </c>
@@ -1008,13 +1163,13 @@
         <v>12</v>
       </c>
       <c r="C46" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="D46" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>47</v>
       </c>
@@ -1022,13 +1177,13 @@
         <v>12</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="D47" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4">
       <c r="A48">
         <v>48</v>
       </c>
@@ -1036,13 +1191,13 @@
         <v>12</v>
       </c>
       <c r="C48" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="D48" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49">
         <v>49</v>
       </c>
@@ -1050,13 +1205,13 @@
         <v>13</v>
       </c>
       <c r="C49" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="D49" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50">
         <v>50</v>
       </c>
@@ -1064,13 +1219,13 @@
         <v>13</v>
       </c>
       <c r="C50" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="D50" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51">
         <v>51</v>
       </c>
@@ -1078,13 +1233,13 @@
         <v>13</v>
       </c>
       <c r="C51" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="D51" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52">
         <v>52</v>
       </c>
@@ -1092,13 +1247,13 @@
         <v>13</v>
       </c>
       <c r="C52" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="D52" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53">
         <v>53</v>
       </c>
@@ -1106,13 +1261,13 @@
         <v>14</v>
       </c>
       <c r="C53" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="D53" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54">
         <v>54</v>
       </c>
@@ -1120,13 +1275,13 @@
         <v>14</v>
       </c>
       <c r="C54" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="D54" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55">
         <v>55</v>
       </c>
@@ -1134,13 +1289,13 @@
         <v>14</v>
       </c>
       <c r="C55" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="D55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56">
         <v>56</v>
       </c>
@@ -1148,13 +1303,13 @@
         <v>14</v>
       </c>
       <c r="C56" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="D56" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4">
       <c r="A57">
         <v>57</v>
       </c>
@@ -1162,13 +1317,13 @@
         <v>15</v>
       </c>
       <c r="C57" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="D57" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4">
       <c r="A58">
         <v>58</v>
       </c>
@@ -1176,13 +1331,13 @@
         <v>15</v>
       </c>
       <c r="C58" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="D58" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4">
       <c r="A59">
         <v>59</v>
       </c>
@@ -1190,13 +1345,13 @@
         <v>15</v>
       </c>
       <c r="C59" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="D59" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4">
       <c r="A60">
         <v>60</v>
       </c>
@@ -1204,13 +1359,13 @@
         <v>15</v>
       </c>
       <c r="C60" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D60" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4">
       <c r="A61">
         <v>61</v>
       </c>
@@ -1224,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4">
       <c r="A62">
         <v>62</v>
       </c>
@@ -1238,7 +1393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4">
       <c r="A63">
         <v>63</v>
       </c>
@@ -1252,7 +1407,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4">
       <c r="A64">
         <v>64</v>
       </c>
@@ -1266,7 +1421,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4">
       <c r="A65">
         <v>65</v>
       </c>
@@ -1280,7 +1435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4">
       <c r="A66">
         <v>66</v>
       </c>
@@ -1294,7 +1449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4">
       <c r="A67">
         <v>67</v>
       </c>
@@ -1308,7 +1463,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4">
       <c r="A68">
         <v>68</v>
       </c>
@@ -1322,7 +1477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4">
       <c r="A69">
         <v>69</v>
       </c>
@@ -1336,7 +1491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4">
       <c r="A70">
         <v>70</v>
       </c>
@@ -1350,7 +1505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4">
       <c r="A71">
         <v>71</v>
       </c>
@@ -1364,7 +1519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4">
       <c r="A72">
         <v>72</v>
       </c>
@@ -1378,7 +1533,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4">
       <c r="A73">
         <v>73</v>
       </c>
@@ -1392,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4">
       <c r="A74">
         <v>74</v>
       </c>
@@ -1406,7 +1561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4">
       <c r="A75">
         <v>75</v>
       </c>
@@ -1420,7 +1575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4">
       <c r="A76">
         <v>76</v>
       </c>
@@ -1434,7 +1589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4">
       <c r="A77">
         <v>77</v>
       </c>
@@ -1448,7 +1603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4">
       <c r="A78">
         <v>78</v>
       </c>
@@ -1462,7 +1617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4">
       <c r="A79">
         <v>79</v>
       </c>
@@ -1476,7 +1631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4">
       <c r="A80">
         <v>80</v>
       </c>
@@ -1492,5 +1647,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>